<commit_message>
implemented the twilio in the leadGathering
</commit_message>
<xml_diff>
--- a/Sales_Leads.xlsx
+++ b/Sales_Leads.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Timestamp</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>PhoneNumber</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -476,6 +481,7 @@
           <t>2025-10-31 16:25:01</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -498,6 +504,7 @@
           <t>2025-10-31 16:26:37</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -520,6 +527,7 @@
           <t>2025-10-31 16:29:01</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -542,6 +550,7 @@
           <t>2025-10-31 16:30:21</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -564,6 +573,7 @@
           <t>2025-10-31 16:35:07</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -586,6 +596,7 @@
           <t>2025-10-31 16:36:03</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -606,6 +617,34 @@
       <c r="D8" t="inlineStr">
         <is>
           <t>2025-10-31 17:09:02</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Batman.</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Interested</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-11-04 17:39:01</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>+919510038048</t>
         </is>
       </c>
     </row>

</xml_diff>